<commit_message>
Breakdown of box Datasets folder
</commit_message>
<xml_diff>
--- a/Dashboard/Survey_compilation.xlsx
+++ b/Dashboard/Survey_compilation.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="104">
   <si>
     <t>Country</t>
   </si>
@@ -236,9 +236,6 @@
     <t>.SAV</t>
   </si>
   <si>
-    <t>Misc</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 2 - different weighting</t>
   </si>
   <si>
@@ -251,9 +248,6 @@
     <t>n</t>
   </si>
   <si>
-    <t>zip</t>
-  </si>
-  <si>
     <t>Change logs</t>
   </si>
   <si>
@@ -287,10 +281,64 @@
     <t>3 PDFs of questions</t>
   </si>
   <si>
-    <t>1 PDF</t>
-  </si>
-  <si>
     <t>2 PDFs</t>
+  </si>
+  <si>
+    <t>1 PDF (Espanol version)</t>
+  </si>
+  <si>
+    <t>zip (.dat + .sav)</t>
+  </si>
+  <si>
+    <t>2 + 2 "…Rev1-w.zip"</t>
+  </si>
+  <si>
+    <t>1PDF "2006_v23ER.pdf"</t>
+  </si>
+  <si>
+    <t>1 PDF (2006_v23)</t>
+  </si>
+  <si>
+    <t>2 PDFs (2008 18Q_jan2308_V2 revised.pdf &amp; 2006_v23CR.pdf)</t>
+  </si>
+  <si>
+    <t>2 PDFs (2006_v23iR.pdf &amp; Spanish V18Q_V2 revised.pdf)</t>
+  </si>
+  <si>
+    <t>2 PDFs (Spanish v18Q_V2 revised.pdf &amp; 2006_v23b.pdf)</t>
+  </si>
+  <si>
+    <t>2 PDFs (2006_v23_BR.pdf &amp; Spanish V18Qr_V2 revised.pdf)</t>
+  </si>
+  <si>
+    <t>2 PDFs (2006_v23bR1.pdf &amp; Spanish v18Q_V2 revised.pdf)</t>
+  </si>
+  <si>
+    <t>2 PDFs (Spanish V18Q_V2 revised.pdf &amp; 2006_v23bR1.pdf)</t>
+  </si>
+  <si>
+    <t>1 PDF (Spanish V18Q_V2 revised.pdf)</t>
+  </si>
+  <si>
+    <t>2 PDFs (Spanish v18p_V2 revised.pdf &amp; 2006_v23G-1R.pdf)</t>
+  </si>
+  <si>
+    <t>2010-2014</t>
+  </si>
+  <si>
+    <t>2 PDFs (Spanish_v18Q9_V2 revised.pdf &amp; Uruguay2007_v9 _3_.pdf)</t>
+  </si>
+  <si>
+    <t>2 PDFs (Spanish_V15R_V2 revised.pdf &amp; Venezuela_v12.pdf)</t>
+  </si>
+  <si>
+    <t>1 PDF (Spanish_v18Q_V2 revised.pdf)</t>
+  </si>
+  <si>
+    <t>1 (.sav)</t>
+  </si>
+  <si>
+    <t>Misc (some of these PDFs could be questionaires)</t>
   </si>
 </sst>
 </file>
@@ -326,10 +374,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -610,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -623,8 +674,9 @@
     <col min="5" max="5" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="52.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="56.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -647,7 +699,7 @@
         <v>37</v>
       </c>
       <c r="G1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H1" t="s">
         <v>67</v>
@@ -656,16 +708,16 @@
         <v>68</v>
       </c>
       <c r="J1" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="K1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M1" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -682,7 +734,7 @@
         <v>66</v>
       </c>
       <c r="G2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -702,10 +754,10 @@
         <v>39</v>
       </c>
       <c r="E3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" t="s">
         <v>71</v>
-      </c>
-      <c r="F3" t="s">
-        <v>72</v>
       </c>
       <c r="G3">
         <v>5</v>
@@ -762,6 +814,15 @@
       <c r="C5" s="1">
         <v>14</v>
       </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -774,10 +835,10 @@
         <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -798,7 +859,7 @@
         <v>2</v>
       </c>
       <c r="M6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -815,7 +876,7 @@
         <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F7" t="str">
         <f>IF(H7&lt;B7, "n", "y")</f>
@@ -840,7 +901,7 @@
         <v>2</v>
       </c>
       <c r="M7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -854,7 +915,7 @@
         <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F8" t="str">
         <f>IF(H8&lt;B8, "n", "y")</f>
@@ -876,7 +937,7 @@
         <v>2</v>
       </c>
       <c r="M8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -890,7 +951,7 @@
         <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F9" t="str">
         <f>IF(H9&lt;B9, "n", "y")</f>
@@ -915,7 +976,7 @@
         <v>2</v>
       </c>
       <c r="M9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -929,7 +990,11 @@
         <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>83</v>
+        <v>81</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" ref="F10:F17" si="0">IF(H10&lt;B10, "n", "y")</f>
+        <v>y</v>
       </c>
       <c r="G10">
         <v>6</v>
@@ -950,7 +1015,7 @@
         <v>2</v>
       </c>
       <c r="M10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -964,7 +1029,11 @@
         <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>y</v>
       </c>
       <c r="G11">
         <v>13</v>
@@ -985,7 +1054,7 @@
         <v>2</v>
       </c>
       <c r="M11" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -1002,7 +1071,11 @@
         <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
       </c>
       <c r="G12">
         <v>7</v>
@@ -1023,7 +1096,7 @@
         <v>2</v>
       </c>
       <c r="M12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1036,6 +1109,19 @@
       <c r="C13" s="1">
         <v>16</v>
       </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>y</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1048,7 +1134,11 @@
         <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
       </c>
       <c r="G14">
         <v>5</v>
@@ -1069,7 +1159,7 @@
         <v>2</v>
       </c>
       <c r="M14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -1085,6 +1175,34 @@
       <c r="D15" t="s">
         <v>47</v>
       </c>
+      <c r="E15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+      <c r="G15">
+        <v>6</v>
+      </c>
+      <c r="H15">
+        <v>7</v>
+      </c>
+      <c r="I15">
+        <v>6</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <v>4</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1099,8 +1217,36 @@
       <c r="D16" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+      <c r="G16">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <v>7</v>
+      </c>
+      <c r="I16">
+        <v>6</v>
+      </c>
+      <c r="J16" t="s">
+        <v>87</v>
+      </c>
+      <c r="K16">
+        <v>3</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1110,8 +1256,21 @@
       <c r="C17" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>y</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1124,8 +1283,36 @@
       <c r="D18" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" t="str">
+        <f>IF(H18&lt;B18, "n", "y")</f>
+        <v>n</v>
+      </c>
+      <c r="G18">
+        <v>6</v>
+      </c>
+      <c r="H18">
+        <v>8</v>
+      </c>
+      <c r="I18">
+        <v>6</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <v>2</v>
+      </c>
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1135,8 +1322,36 @@
       <c r="C19" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" t="str">
+        <f>IF(H19&lt;B19, "n", "y")</f>
+        <v>y</v>
+      </c>
+      <c r="G19">
+        <v>7</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+      <c r="I19">
+        <v>6</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
+      <c r="L19">
+        <v>2</v>
+      </c>
+      <c r="M19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1146,8 +1361,33 @@
       <c r="C20" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" t="str">
+        <f>IF(H20&lt;B20, "n", "y")</f>
+        <v>y</v>
+      </c>
+      <c r="G20">
+        <v>6</v>
+      </c>
+      <c r="H20">
+        <v>6</v>
+      </c>
+      <c r="I20">
+        <v>5</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
+      </c>
+      <c r="K20">
+        <v>2</v>
+      </c>
+      <c r="L20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1160,8 +1400,36 @@
       <c r="D21" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" t="str">
+        <f>IF(H21&lt;B21, "n", "y")</f>
+        <v>n</v>
+      </c>
+      <c r="G21">
+        <v>7</v>
+      </c>
+      <c r="H21">
+        <v>7</v>
+      </c>
+      <c r="I21">
+        <v>6</v>
+      </c>
+      <c r="J21">
+        <v>2</v>
+      </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="L21">
+        <v>2</v>
+      </c>
+      <c r="M21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1171,8 +1439,36 @@
       <c r="C22" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" t="str">
+        <f>IF(H22&lt;B22, "n", "y")</f>
+        <v>y</v>
+      </c>
+      <c r="G22">
+        <v>6</v>
+      </c>
+      <c r="H22">
+        <v>6</v>
+      </c>
+      <c r="I22">
+        <v>5</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
+      </c>
+      <c r="M22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1185,8 +1481,36 @@
       <c r="D23" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" t="str">
+        <f>IF(H23&lt;B23, "n", "y")</f>
+        <v>n</v>
+      </c>
+      <c r="G23">
+        <v>7</v>
+      </c>
+      <c r="H23">
+        <v>7</v>
+      </c>
+      <c r="I23">
+        <v>6</v>
+      </c>
+      <c r="J23">
+        <v>2</v>
+      </c>
+      <c r="K23">
+        <v>2</v>
+      </c>
+      <c r="L23">
+        <v>2</v>
+      </c>
+      <c r="M23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1196,8 +1520,36 @@
       <c r="C24" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>77</v>
+      </c>
+      <c r="F24" t="str">
+        <f>IF(H24&lt;B24, "n", "y")</f>
+        <v>n</v>
+      </c>
+      <c r="G24">
+        <v>7</v>
+      </c>
+      <c r="H24">
+        <v>7</v>
+      </c>
+      <c r="I24">
+        <v>6</v>
+      </c>
+      <c r="J24">
+        <v>2</v>
+      </c>
+      <c r="K24">
+        <v>2</v>
+      </c>
+      <c r="L24">
+        <v>2</v>
+      </c>
+      <c r="M24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1210,8 +1562,36 @@
       <c r="D25" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>77</v>
+      </c>
+      <c r="F25" t="str">
+        <f>IF(H25&lt;B25, "n", "y")</f>
+        <v>n</v>
+      </c>
+      <c r="G25">
+        <v>7</v>
+      </c>
+      <c r="H25">
+        <v>7</v>
+      </c>
+      <c r="I25">
+        <v>6</v>
+      </c>
+      <c r="J25">
+        <v>2</v>
+      </c>
+      <c r="K25">
+        <v>2</v>
+      </c>
+      <c r="L25">
+        <v>2</v>
+      </c>
+      <c r="M25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1221,8 +1601,36 @@
       <c r="C26" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" t="str">
+        <f>IF(H26&lt;B26, "n", "y")</f>
+        <v>n</v>
+      </c>
+      <c r="G26">
+        <v>6</v>
+      </c>
+      <c r="H26">
+        <v>6</v>
+      </c>
+      <c r="I26">
+        <v>5</v>
+      </c>
+      <c r="J26">
+        <v>2</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>2</v>
+      </c>
+      <c r="M26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1232,8 +1640,36 @@
       <c r="C27" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
+        <v>81</v>
+      </c>
+      <c r="F27" t="str">
+        <f>IF(H27&lt;B27, "n", "y")</f>
+        <v>n</v>
+      </c>
+      <c r="G27">
+        <v>6</v>
+      </c>
+      <c r="H27">
+        <v>7</v>
+      </c>
+      <c r="I27">
+        <v>5</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>2</v>
+      </c>
+      <c r="M27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1243,8 +1679,21 @@
       <c r="C28" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F28" t="str">
+        <f>IF(H28&lt;B28, "n", "y")</f>
+        <v>y</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1254,8 +1703,21 @@
       <c r="C29" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F29" t="str">
+        <f>IF(H29&lt;B29, "n", "y")</f>
+        <v>y</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1265,8 +1727,21 @@
       <c r="C30" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F30" t="str">
+        <f>IF(H30&lt;B30, "n", "y")</f>
+        <v>y</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1276,8 +1751,29 @@
       <c r="C31" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>98</v>
+      </c>
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="H31">
+        <v>3</v>
+      </c>
+      <c r="I31">
+        <v>3</v>
+      </c>
+      <c r="J31">
+        <v>2</v>
+      </c>
+      <c r="K31">
+        <v>2</v>
+      </c>
+      <c r="L31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1287,8 +1783,29 @@
       <c r="C32" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>98</v>
+      </c>
+      <c r="G32">
+        <v>3</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>2</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1298,8 +1815,29 @@
       <c r="C33" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E33" t="s">
+        <v>81</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>3</v>
+      </c>
+      <c r="I33">
+        <v>2</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+      <c r="K33">
+        <v>2</v>
+      </c>
+      <c r="L33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1309,8 +1847,32 @@
       <c r="C34" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G34">
+        <v>6</v>
+      </c>
+      <c r="H34">
+        <v>6</v>
+      </c>
+      <c r="I34">
+        <v>5</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>2</v>
+      </c>
+      <c r="M34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1319,6 +1881,30 @@
       </c>
       <c r="C35" s="1" t="s">
         <v>64</v>
+      </c>
+      <c r="E35" t="s">
+        <v>79</v>
+      </c>
+      <c r="G35">
+        <v>6</v>
+      </c>
+      <c r="H35">
+        <v>6</v>
+      </c>
+      <c r="I35">
+        <v>5</v>
+      </c>
+      <c r="J35">
+        <v>2</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>2</v>
+      </c>
+      <c r="M35" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Additional files, file counts and formatting
</commit_message>
<xml_diff>
--- a/Dashboard/Survey_compilation.xlsx
+++ b/Dashboard/Survey_compilation.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="293">
   <si>
     <t>Country</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Trinidad and Tobago</t>
   </si>
   <si>
-    <t>USA</t>
-  </si>
-  <si>
     <t>Uruguay</t>
   </si>
   <si>
@@ -251,9 +248,6 @@
     <t>Change logs</t>
   </si>
   <si>
-    <t>tech report</t>
-  </si>
-  <si>
     <t>Files on box: TECH INFO</t>
   </si>
   <si>
@@ -339,13 +333,586 @@
   </si>
   <si>
     <t>Misc (some of these PDFs could be questionaires)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Additional</t>
+  </si>
+  <si>
+    <t>55186908VAND0002_CODEBOOK.pdf</t>
+  </si>
+  <si>
+    <t>2128470678US CODEBOOK.pdf</t>
+  </si>
+  <si>
+    <t>various w.zip folders</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AB Tech Info</t>
+  </si>
+  <si>
+    <t>"Brasil" tech info</t>
+  </si>
+  <si>
+    <t>"Dom Rep" tech info</t>
+  </si>
+  <si>
+    <t>11842458662004_Core_Questionnaire_English.pdf</t>
+  </si>
+  <si>
+    <t>590988561ABUS12-v10.0.1.2-Eng-Online Survey-120409_W.pdf</t>
+  </si>
+  <si>
+    <t>498336009US_LAPOP_AmericasBarometer 2010 data set original V1.sav</t>
+  </si>
+  <si>
+    <t>4052167482006_Core_Questionnaire_English.pdf</t>
+  </si>
+  <si>
+    <t>1332767016Belice_LAPOP_AmericasBarometer 2010 data set approved v3.dta</t>
+  </si>
+  <si>
+    <t>20574795612004_Core_Questionnaire_Spanish.pdf</t>
+  </si>
+  <si>
+    <t>11894059352008_Core_Questionnaire_English.pdf</t>
+  </si>
+  <si>
+    <t>106588472008_Core_Questionnaire_Spanish.pdf</t>
+  </si>
+  <si>
+    <t>726824552010_Core_Questionnaire_English.pdf</t>
+  </si>
+  <si>
+    <t>982888672Belice_LAPOP_AmericasBarometer 2010 data set approved v3.sav</t>
+  </si>
+  <si>
+    <t>496679067TrinandTob LAPOP AmericasBarometer 2012 Rev1_W.dta</t>
+  </si>
+  <si>
+    <t>14423965852006_Core_Questionnaire_Spanish.pdf</t>
+  </si>
+  <si>
+    <t>1369231269ABCan17-v18.0.6.1-Fre-Online-Survey-170323_W.pdf</t>
+  </si>
+  <si>
+    <t>1788592306ABCan17-v18.0.6.1-Eng-Online-Survey-170323_W.pdf</t>
+  </si>
+  <si>
+    <t>1076064826DomRep LAPOP AmericasBarometer 2012 Rev1_W.dta</t>
+  </si>
+  <si>
+    <t>1055323533USA LAPOP 2008 FINAL DATASET_v10.sav</t>
+  </si>
+  <si>
+    <t>1274325220ABCan12-V10.0.4.0-Eng-Online Survey-120713_W.pdf</t>
+  </si>
+  <si>
+    <t>1564237303dr_lapop_final 2006 data set v2.dta</t>
+  </si>
+  <si>
+    <t>356764203ABSur12-v10.0.2.2-Sra-120427_W.pdf</t>
+  </si>
+  <si>
+    <t>872527770ABUS17-v18.0.3.1-Spa-Online Survey-170515_W.pdf</t>
+  </si>
+  <si>
+    <t>1873964806ABCan12-V10.0.4.0-FRE-Online Survey-120716_W.pdf</t>
+  </si>
+  <si>
+    <t>861125112DR_LAPOP_Final 2006 data set V2.sav</t>
+  </si>
+  <si>
+    <t>400811956LAPOPUS14-V15.2.5.2-Eng-Online_Survey-140604_W.pdf</t>
+  </si>
+  <si>
+    <t>1932825432LAPOPUS14-V15.2.5.2-Spa-Online_Survey-140612_W.pdf</t>
+  </si>
+  <si>
+    <t>1929200576LAPOPArg14-V15.2.3.0-Spa-140218_W.pdf</t>
+  </si>
+  <si>
+    <t>302018996ABBol17-v18.0.4.1-Spa-170601_W.pdf</t>
+  </si>
+  <si>
+    <t>2055947480Ayiti_LAPOP_DIMS_2008_v18Qi_V2_revised.pdf</t>
+  </si>
+  <si>
+    <t>1687107686Ayiti_LAPOP_DIMS_2008_v18Qi_V2 revised.pdf</t>
+  </si>
+  <si>
+    <t>1998926922LAPOP DIMS 2008 core English USA v10_V2 revised.pdf</t>
+  </si>
+  <si>
+    <t>265338482LAPOPBra14-v15.2.5.1-Por-140316_W.pdf</t>
+  </si>
+  <si>
+    <t>1988909161LAPOPHai14-V15.2.3.1-Creole-140214_W.pdf</t>
+  </si>
+  <si>
+    <t>293937906ABHai17-v18.0.5.0-Creole-170406_W.pdf</t>
+  </si>
+  <si>
+    <t>1602603624ABHai17-v18.0.4.0-Eng-170406_W.pdf</t>
+  </si>
+  <si>
+    <t>15468202082004-2014 Grand Merge Codebook_V3.0_Free_W.pdf</t>
+  </si>
+  <si>
+    <t>16345650682004 - 2014 Grand Merge Codebook_V3.0_W.pdf</t>
+  </si>
+  <si>
+    <t>1126299224LAPOPGuy14-v15.2.3.1-Eng-140530_W.pdf</t>
+  </si>
+  <si>
+    <t>1738442662LAPOPBel14-V15.2.2.2-Eng-140501_W.pdf</t>
+  </si>
+  <si>
+    <t>1758247732LAPOPNic14-v15.2.7.0-Spa-140212_W.pdf</t>
+  </si>
+  <si>
+    <t>523612957LAPOPRep14-v15.2.2.0-Spa-140201_W.pd</t>
+  </si>
+  <si>
+    <t>848604546LAPOPBol14-v15.2.3.2-Spa-140323_W.pdf</t>
+  </si>
+  <si>
+    <t>1962881277LAPOPVen14-v15.2.3.2-Spa-140221_W.pdf</t>
+  </si>
+  <si>
+    <t>269582202TrinandTob LAPOP AmericasBarometer 2012 Rev1_W.sav</t>
+  </si>
+  <si>
+    <t>1266704853LAPOPBel14-v15.2.2.0-Spa-140428_W.pdf</t>
+  </si>
+  <si>
+    <t>1760030174LAPOPPar14-V15.2.4.3-Spa-Gua-140116_W.pdf</t>
+  </si>
+  <si>
+    <t>833646236LAPOPEcu14-15.2.5.1-Spa-140117_W.pdf</t>
+  </si>
+  <si>
+    <t>746535198LAPOPPan14-v15.2.3.0-Spa-131218_W.pdf</t>
+  </si>
+  <si>
+    <t>584811784LAPOPChi14-v15.2.3.2-Spa-140329_W.pdf</t>
+  </si>
+  <si>
+    <t>1117676277LAPOPBar14-V15.2.6.2-Eng-150219_W.pdf</t>
+  </si>
+  <si>
+    <t>587141161LAPOPPer14-v15.2.3.5-Spa-140122_W_A4.pdf</t>
+  </si>
+  <si>
+    <t>879123266LAPOPUru14-V15.2.4.2-Spa-140324_W.pdf</t>
+  </si>
+  <si>
+    <t>1139038545LAPOPBol14-v15.2.3.2-Quechua-140323_W.pdf</t>
+  </si>
+  <si>
+    <t>2034734982LAPOPBah14-V15.2.4.1-Eng-140612_W.pdf</t>
+  </si>
+  <si>
+    <t>1106119498LAPOPDca16-V15.2.4.2-Eng-160112_W.pdf</t>
+  </si>
+  <si>
+    <t>2003571071LAPOPBol14-v15.2.3.2-Aym-140323_W.pdf</t>
+  </si>
+  <si>
+    <t>354247926LAPOPSur14-V15.2.4.4-Sra-140617_W.pdf</t>
+  </si>
+  <si>
+    <t>386410555LAPOPStl16-V15.2.4.4-Eng-160201_W.pdf</t>
+  </si>
+  <si>
+    <t>1617641174LAPOPStk16-V15.2.4.2-Eng-151216_W.pdf</t>
+  </si>
+  <si>
+    <t>1125739622LAPOPAnt16-V15.2.4.2-Eng-151216_W.pdf</t>
+  </si>
+  <si>
+    <t>1685157827ABPer17-v18.0.11.1-Spa-170203_W.pdf</t>
+  </si>
+  <si>
+    <t>288530685LAPOPCos14-v15.2.2.2-Spa-140219_W.pdf</t>
+  </si>
+  <si>
+    <t>905691160LAPOPStv16-V15.2.4.2-Eng-151217_W.pdf</t>
+  </si>
+  <si>
+    <t>783073873LAPOPGre16-V15.2.4.3-Eng-151216_W.pdf</t>
+  </si>
+  <si>
+    <t>1034661191LAPOPSur14-v15.2.4.4-Dut-140619_W.pdf</t>
+  </si>
+  <si>
+    <t>445177969LAPOPMex14-v15.2.2.1-Spa-140114_W.pdf</t>
+  </si>
+  <si>
+    <t>889703241LAPOPHai14-v15.2.3.1-Eng-140214_W.pdf </t>
+  </si>
+  <si>
+    <t>12364388022004-2014 Grand Merge Codebook_V3.0_Free_W.pdf </t>
+  </si>
+  <si>
+    <t>1054197763ABUS12-v10.0.1.2-Spa-Online Survey-120409_W.pdf </t>
+  </si>
+  <si>
+    <t>15679094712010_Core_Questionnaire_SPANISH.pdf </t>
+  </si>
+  <si>
+    <t>651425998ABSur12-v10.0.2.4-Dut-120425_W.pdf </t>
+  </si>
+  <si>
+    <t>1435084394ABSur12-v10.0.2.2-Eng-120425_W.pdf </t>
+  </si>
+  <si>
+    <t>664841849LAPOPCan14-V15.2.2.0-Eng-Online_Survey-140620_W.pdf </t>
+  </si>
+  <si>
+    <t>1030308463LAPOPCan14-V15.2.2.0-Fre-Online_Survey-140828_W.pdf </t>
+  </si>
+  <si>
+    <t>1295912352ABUS17-v18.0.3.1-Eng-Online Survey-170504_W.pdf </t>
+  </si>
+  <si>
+    <t>1938999605ABHai12-V9.1.4.0-Eng-120104_VF_W.pdf </t>
+  </si>
+  <si>
+    <t>1409537476ABHai12-V9.1.4.0-Creole-120104_VF_W.pdf </t>
+  </si>
+  <si>
+    <t>1473291271LAPOPSur14-V15.2.4.2-Eng-140515_W.pdf </t>
+  </si>
+  <si>
+    <t>817947147LAPOPGua14-v15.2.5.1-Spa-140327_W.pdf </t>
+  </si>
+  <si>
+    <t>1180652188ABGuy12-v10.0.3.1-Eng-120118_W.pdf </t>
+  </si>
+  <si>
+    <t>1091542633LAPOP2014-v15.2-Eng-131218_W.pdf </t>
+  </si>
+  <si>
+    <t>63622196ABJam12-v10.0.2.1-Eng-120210_W.pdf </t>
+  </si>
+  <si>
+    <t>1052038031ABVen16-v14.0.2.6-Spa-170105_W.pdf </t>
+  </si>
+  <si>
+    <t>1088204337ABEcu16-v14.0.7.1-Spa-161107_W.pdf </t>
+  </si>
+  <si>
+    <t>1945870122DomRep LAPOP AmericasBarometer 2012 Rev1_W.sav </t>
+  </si>
+  <si>
+    <t>1970520867LAPOPGuy16-V15.2.6.0-Eng-160303_W.pdf </t>
+  </si>
+  <si>
+    <t>2035948080LAPOP2014-v15.2-Spa-131218_W.pdf </t>
+  </si>
+  <si>
+    <t>664264584LAPOPTri14-V15.2.4.1-Eng-140308_W.pdf </t>
+  </si>
+  <si>
+    <t>713700907ABBel12-v10.0.1.1-Eng-120306_W.pdf </t>
+  </si>
+  <si>
+    <t>844128648LAPOPHon14-v15.2.3.1-Spa-140314_W.pdf </t>
+  </si>
+  <si>
+    <t>571265452LAPOPEls14-v15.2.2.3-Spa-140325_W.pdf </t>
+  </si>
+  <si>
+    <t>446681011ABBel12-v10.0.1.2-Spa-120313_W.pdf </t>
+  </si>
+  <si>
+    <t>1461505070ABBol12-V10.0.2.1-Quechua-120508_W.pdf </t>
+  </si>
+  <si>
+    <t>1503287022ABRep16-v14.0.3.2-Spa-170202_W.pdf </t>
+  </si>
+  <si>
+    <t>1707262442ABBol12-v10.0.2.1-Spa-120223_W.pdf </t>
+  </si>
+  <si>
+    <t>781837751ABTri12-V10.0.2.2-Eng-120320_W.pdf </t>
+  </si>
+  <si>
+    <t>763622927ABEcu12-v10.0.1.0-Spa-120127_W.pdf </t>
+  </si>
+  <si>
+    <t>1171133318LAPOPJam14-v15.2.4.3-Eng-140220_W.pdf </t>
+  </si>
+  <si>
+    <t>1859565254ABBol12-V10.0.2.1-Aym-120430_W.pdf </t>
+  </si>
+  <si>
+    <t>1894672119ABNic16-v13.0.3.3-Spa-160913_W.pdf </t>
+  </si>
+  <si>
+    <t>1788509698ABPan12-v10.0.3.0-Spa-120125_W.pdf </t>
+  </si>
+  <si>
+    <t>293224884ABCos16-v11.0.5.0-Spa-160816_W.pdf </t>
+  </si>
+  <si>
+    <t>1100557450ABJam17-v18.0.3.2-Eng-170213_W.pdf </t>
+  </si>
+  <si>
+    <t>1727039552ABMex17-v16.0.2.1-Spa-170130_W.pdf </t>
+  </si>
+  <si>
+    <t>102476357ABPar16-v14.0.6.4-Spa-Gua-161102_W.pdf </t>
+  </si>
+  <si>
+    <t>469847136ABPar16-v14.0.6.4-Spa-Gua-161102_W.pdf </t>
+  </si>
+  <si>
+    <t>444292633ABNic12-v10.0.1.3-Spa-120201_W.pdf </t>
+  </si>
+  <si>
+    <t>1053282920ABArg12-v10.0.3.3-Spa-120228_W.pdf </t>
+  </si>
+  <si>
+    <t>1927928837ABCos12-v10.0.1.1-Spa-120123_W.pdf </t>
+  </si>
+  <si>
+    <t>311691868ABUru12-v10.0.4.1-Spa-120301_W.pdf </t>
+  </si>
+  <si>
+    <t>260793346ABArg17-v18.0.7.0-Spa-170307_W.pdf </t>
+  </si>
+  <si>
+    <t>291055575ABRep12-v10.0.3.0-Spa-120130_W.pdf </t>
+  </si>
+  <si>
+    <t>18017015502010_Belice_Cuestionario.pdf </t>
+  </si>
+  <si>
+    <t>1198371617ABBra12-v10.0.2.6-Por-120722_W.pdf </t>
+  </si>
+  <si>
+    <t>43821536ABCor12-v10.0-Eng-120222_W.pdf </t>
+  </si>
+  <si>
+    <t>1381977883ABGua12-v10.0.2.1-Spa-120311_W.pdf </t>
+  </si>
+  <si>
+    <t>563786593ABCor12-v10.0-Spa-120117_W.pdf </t>
+  </si>
+  <si>
+    <t>1054347574ABGua17-v18.0.2.0-Spa-170214_W.pdf </t>
+  </si>
+  <si>
+    <t>1121386762ABChi12-v10.0.3.2-Spa-120307_W.pdf </t>
+  </si>
+  <si>
+    <t>1742690002LAPOPCol14-v15.2.3.0-Spa-140325_W.pdf </t>
+  </si>
+  <si>
+    <t>1807407256ABMex12-v10.0.2.0-Spa-120118_W.pdf </t>
+  </si>
+  <si>
+    <t>1800498527ABEcu12-v10.0.1.3-Kichwa-120210_W.pdf </t>
+  </si>
+  <si>
+    <t>1958371786ABGua12-v10.0.2.0-Kiche-120308_W.pdf </t>
+  </si>
+  <si>
+    <t>930147908ABGua12-v10.0.2.0-Kiche-120308_W.pdf </t>
+  </si>
+  <si>
+    <t>1580960269ABPar12-V10.0.1.1-Spa-Gua-120201_W.pdf </t>
+  </si>
+  <si>
+    <t>1471843171ABHon12-v10.0.2.1-Spa-120118_W.pdf </t>
+  </si>
+  <si>
+    <t>384743331ABHon16-v14.0.5.0-Spa-161013_W.pdf </t>
+  </si>
+  <si>
+    <t>596424100ABVen12-v10.0.2.3-Spa-120403_W.pdf </t>
+  </si>
+  <si>
+    <t>1486390985Ayiti_LAPOP_DIMS_2006_v23.pdf </t>
+  </si>
+  <si>
+    <t>678857426ABEls12-v10.0.4.1-Spa-120405_W.pdf </t>
+  </si>
+  <si>
+    <t>410218884ABGua12-v10.0.2.0-Qeqchi-120309_W.pdf </t>
+  </si>
+  <si>
+    <t>1275069098ABPer12-v9.1.1.1-Spa-120113_A4(5)_W.pdf </t>
+  </si>
+  <si>
+    <t>1177283467ABEls16-v14.0.2.2-Spa-161023_W.pdf </t>
+  </si>
+  <si>
+    <t>17600748482010_Brasil_Questionnaire_Portuguese.pdf </t>
+  </si>
+  <si>
+    <t>1293954103ABCor04-12-Spa_Grand Merge_Free_Rev1_W.pdf </t>
+  </si>
+  <si>
+    <t>1084775958ABCor04-12-Spa_Grand Merge_Rev1_W.pdf </t>
+  </si>
+  <si>
+    <t>373577961ABCol12-v10.0.5.0-Spa-120316_W.pdf </t>
+  </si>
+  <si>
+    <t>389170919LAPOP_Brasil_Final_Questionnaire.pdf </t>
+  </si>
+  <si>
+    <t>753391186ABCor04-12-Spa_Grand-Merge_W.pdf </t>
+  </si>
+  <si>
+    <t>1346452956ABCor04-12-Spa_Grand-Merge_Free_W.pdf </t>
+  </si>
+  <si>
+    <t>1604359859ABPan17-v18.0.2.2-Spa-170217_W.pdf </t>
+  </si>
+  <si>
+    <t>215774101ABBra17-v18.0.5.6-Por-170410_W.pdf </t>
+  </si>
+  <si>
+    <t>1774629649ABCol2016-v9.0.5.2-Spa-160802_W.pdf </t>
+  </si>
+  <si>
+    <t>158845851ABChi17-v18.0.6.0-Spa-170411_W.pdf </t>
+  </si>
+  <si>
+    <t>216680056ABUru17-v18.0.4.0-Spa-170314_W.pdf </t>
+  </si>
+  <si>
+    <t>533873721AmericasBarometer Merged 2012 English Rev1.5_W_dta.zip </t>
+  </si>
+  <si>
+    <t>1653523819AmericasBarometer Merged 2012 Spanish Rev1.5_W_dta.zip </t>
+  </si>
+  <si>
+    <t>1433762558English_Merge_2010_AmericasBarometer_v14_spssv2.zip </t>
+  </si>
+  <si>
+    <t>118346168barometro_de_las_americas_2004_v7_upload.dta </t>
+  </si>
+  <si>
+    <t>720158497Barometro de las Americas 2004 v6 upload.sav </t>
+  </si>
+  <si>
+    <t>765634716AmericasBarometer Merged 2014 v3.0_W_dta.zip </t>
+  </si>
+  <si>
+    <t>1261849700AmericasBarometer Merged 2014 v3.0_W_dta.zip </t>
+  </si>
+  <si>
+    <t>1603120541AmericasBarometer Merged 2012 English Rev1.5_W_sav.zip </t>
+  </si>
+  <si>
+    <t>467010732AmericasBarometer Merged 2012 Spanish Rev1.5_W_sav.zip </t>
+  </si>
+  <si>
+    <t>1247855269AmericasBarometer Merged 2014 English v3.0_W_sav.zip </t>
+  </si>
+  <si>
+    <t>677207468AmericasBarometer Merged 2014 Espanol v3.0_W_sav.zip </t>
+  </si>
+  <si>
+    <t>113606129bar_metro_de_las_am_ricas_2006v6.dta </t>
+  </si>
+  <si>
+    <t>737491538Merge_ AB_ 2006 V20_5.sav </t>
+  </si>
+  <si>
+    <t>1509927391AmericasBarometer 2008 to upload v6_1.sav </t>
+  </si>
+  <si>
+    <t>1302324587Barómetro de las Américas 2008 to upload v6_1.sav </t>
+  </si>
+  <si>
+    <t>1488019932AmericasBarometer 2008 to upload v7.dta </t>
+  </si>
+  <si>
+    <t>203284188Barómetro de las Américas 2008 to upload v8.dta </t>
+  </si>
+  <si>
+    <t>884953055merge_2010_bar_metro_de_las_am_ricas_hai_v14v3.dta </t>
+  </si>
+  <si>
+    <t>1626360926english_merge_2010_americasbarometer_v14v3.dta </t>
+  </si>
+  <si>
+    <t>332261038Merge 2010 Barómetro de las Américas Hai v14SPSSv2.sav </t>
+  </si>
+  <si>
+    <t>746278534AmericasBarometer Grand Merge 2004-2014 v3.0_FREE_dta.zip </t>
+  </si>
+  <si>
+    <t>785705945AmericasBarometer Grand Merge 2004-2014 V3.0_W_dta.zip </t>
+  </si>
+  <si>
+    <t>621516204AmericasBarometer Grand Merge 2004-2014 English V3.0_FREE_sav.zip </t>
+  </si>
+  <si>
+    <t>1245467915AmericasBarometer Grand Merge 2004-2014 English V3.0_W_sav.zip </t>
+  </si>
+  <si>
+    <t>AmericasBarometer Grand Merge 2004-2014 v3.0_FREE.dta </t>
+  </si>
+  <si>
+    <t>Grand total</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column5</t>
+  </si>
+  <si>
+    <t>Column6</t>
+  </si>
+  <si>
+    <t>Column7</t>
+  </si>
+  <si>
+    <t>Column8</t>
+  </si>
+  <si>
+    <t>Column9</t>
+  </si>
+  <si>
+    <t>Column10</t>
+  </si>
+  <si>
+    <t>Column11</t>
+  </si>
+  <si>
+    <t>1 tech report</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9 Years04-11-Rev1-w.zip + 1 TS-Rev1-5-w.zip</t>
+  </si>
+  <si>
+    <t>United States</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -353,13 +920,78 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -371,10 +1003,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -382,11 +1030,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="17">
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="40% - Accent2" xfId="2" builtinId="35"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri (Body)"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <name val="Calibri (Body)"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <name val="Calibri (Body)"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <name val="Calibri (Body)"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <name val="Calibri (Body)"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <name val="Calibri (Body)"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -394,6 +1173,43 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Z35" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:Z35"/>
+  <tableColumns count="26">
+    <tableColumn id="1" name="Country"/>
+    <tableColumn id="2" name="Number of datasets online"/>
+    <tableColumn id="3" name="Years (20xx)" dataDxfId="7"/>
+    <tableColumn id="4" name="Comments"/>
+    <tableColumn id="5" name="Merged time-frame on box"/>
+    <tableColumn id="6" name="Years on box (y/n)">
+      <calculatedColumnFormula>IF(H2&lt;B2, "n", "y")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Files on box: TECH INFO"/>
+    <tableColumn id="8" name=".DTA"/>
+    <tableColumn id="9" name=".SAV"/>
+    <tableColumn id="10" name="zip (.dat + .sav)"/>
+    <tableColumn id="11" name="Questionaires/cuestionario"/>
+    <tableColumn id="12" name="Change logs"/>
+    <tableColumn id="13" name="Misc (some of these PDFs could be questionaires)"/>
+    <tableColumn id="14" name="Total"/>
+    <tableColumn id="15" name="Additional"/>
+    <tableColumn id="16" name="Column1" dataDxfId="6"/>
+    <tableColumn id="17" name="Column2"/>
+    <tableColumn id="18" name="Column3" dataDxfId="5"/>
+    <tableColumn id="19" name="Column4"/>
+    <tableColumn id="20" name="Column5" dataDxfId="4"/>
+    <tableColumn id="21" name="Column6"/>
+    <tableColumn id="22" name="Column7" dataDxfId="3"/>
+    <tableColumn id="23" name="Column8"/>
+    <tableColumn id="24" name="Column9" dataDxfId="2"/>
+    <tableColumn id="25" name="Column10"/>
+    <tableColumn id="26" name="Column11" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -659,68 +1475,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:Z38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="P9" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
     <col min="3" max="3" width="61.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
     <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.33203125" customWidth="1"/>
+    <col min="12" max="12" width="13.5" customWidth="1"/>
     <col min="13" max="13" width="56.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" customWidth="1"/>
+    <col min="16" max="16" width="65" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+    <col min="18" max="18" width="57.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" customWidth="1"/>
+    <col min="20" max="20" width="56.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11" customWidth="1"/>
+    <col min="22" max="22" width="47" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" customWidth="1"/>
+    <col min="24" max="24" width="61.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12" customWidth="1"/>
+    <col min="26" max="26" width="69" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" t="s">
         <v>67</v>
       </c>
-      <c r="I1" t="s">
-        <v>68</v>
-      </c>
       <c r="J1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>103</v>
       </c>
+      <c r="P1" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>289</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -731,10 +1600,10 @@
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -742,8 +1611,47 @@
       <c r="I2">
         <v>1</v>
       </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <v>10</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>273</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -751,13 +1659,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
         <v>70</v>
-      </c>
-      <c r="F3" t="s">
-        <v>71</v>
       </c>
       <c r="G3">
         <v>5</v>
@@ -777,8 +1685,48 @@
       <c r="L3">
         <v>2</v>
       </c>
+      <c r="N3">
+        <f>SUM(G3:L3)</f>
+        <v>19</v>
+      </c>
+      <c r="O3">
+        <v>66</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>274</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -789,7 +1737,7 @@
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -803,8 +1751,48 @@
       <c r="L4">
         <v>2</v>
       </c>
+      <c r="N4">
+        <f>SUM(G4:L4)</f>
+        <v>5</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -815,7 +1803,7 @@
         <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -824,10 +1812,50 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="N5">
+        <f>SUM(G5:L5)+1</f>
+        <v>3</v>
+      </c>
+      <c r="O5" s="3">
+        <v>1</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>276</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -835,13 +1863,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -862,10 +1890,50 @@
         <v>2</v>
       </c>
       <c r="M6" t="s">
-        <v>74</v>
+        <v>290</v>
+      </c>
+      <c r="N6">
+        <f>SUM(G6:L6)+1</f>
+        <v>16</v>
+      </c>
+      <c r="O6" s="4">
+        <v>1</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>277</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -873,13 +1941,13 @@
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F7" t="str">
         <f>IF(H7&lt;B7, "n", "y")</f>
@@ -904,10 +1972,44 @@
         <v>2</v>
       </c>
       <c r="M7" t="s">
-        <v>78</v>
+        <v>76</v>
+      </c>
+      <c r="N7">
+        <f>SUM(G7:L7)+1</f>
+        <v>37</v>
+      </c>
+      <c r="O7">
+        <v>7</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>244</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -915,10 +2017,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F8" t="str">
         <f>IF(H8&lt;B8, "n", "y")</f>
@@ -940,10 +2042,43 @@
         <v>2</v>
       </c>
       <c r="M8" t="s">
-        <v>80</v>
+        <v>78</v>
+      </c>
+      <c r="N8">
+        <v>21</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8" s="4" t="s">
+        <v>245</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -951,10 +2086,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F9" t="str">
         <f>IF(H9&lt;B9, "n", "y")</f>
@@ -979,10 +2114,43 @@
         <v>2</v>
       </c>
       <c r="M9" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+      <c r="N9">
+        <v>24</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9" s="4" t="s">
+        <v>246</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -990,10 +2158,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" ref="F10:F17" si="0">IF(H10&lt;B10, "n", "y")</f>
@@ -1018,10 +2186,43 @@
         <v>2</v>
       </c>
       <c r="M10" t="s">
-        <v>83</v>
+        <v>81</v>
+      </c>
+      <c r="N10">
+        <v>25</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10" s="4" t="s">
+        <v>247</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1029,10 +2230,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
@@ -1057,10 +2258,43 @@
         <v>2</v>
       </c>
       <c r="M11" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="N11">
+        <v>51</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="X11" s="4" t="s">
+        <v>248</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1068,13 +2302,13 @@
         <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
@@ -1099,10 +2333,43 @@
         <v>2</v>
       </c>
       <c r="M12" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="N12">
+        <v>30</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
+      </c>
+      <c r="V12" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="X12" s="4" t="s">
+        <v>249</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1125,8 +2392,42 @@
       <c r="I13">
         <v>1</v>
       </c>
+      <c r="N13">
+        <f t="shared" ref="N8:N15" si="1">SUM(G13:L13)</f>
+        <v>4</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+      <c r="V13" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="W13">
+        <v>1</v>
+      </c>
+      <c r="X13" s="4" t="s">
+        <v>250</v>
+      </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1134,10 +2435,10 @@
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
@@ -1162,10 +2463,43 @@
         <v>2</v>
       </c>
       <c r="M14" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="N14">
+        <v>22</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14" s="4" t="s">
+        <v>251</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1173,13 +2507,13 @@
         <v>10</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
         <v>46</v>
       </c>
-      <c r="D15" t="s">
-        <v>47</v>
-      </c>
       <c r="E15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
@@ -1204,10 +2538,43 @@
         <v>2</v>
       </c>
       <c r="M15" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="N15">
+        <v>28</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15" s="4" t="s">
+        <v>252</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1215,13 +2582,13 @@
         <v>10</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
         <v>48</v>
       </c>
-      <c r="D16" t="s">
-        <v>49</v>
-      </c>
       <c r="E16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
@@ -1237,7 +2604,7 @@
         <v>6</v>
       </c>
       <c r="J16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K16">
         <v>3</v>
@@ -1246,10 +2613,43 @@
         <v>2</v>
       </c>
       <c r="M16" t="s">
-        <v>88</v>
+        <v>86</v>
+      </c>
+      <c r="N16">
+        <v>30</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="U16">
+        <v>1</v>
+      </c>
+      <c r="V16" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16" s="4" t="s">
+        <v>253</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1272,8 +2672,41 @@
       <c r="I17">
         <v>1</v>
       </c>
+      <c r="N17">
+        <v>30</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="W17">
+        <v>1</v>
+      </c>
+      <c r="X17" s="4" t="s">
+        <v>254</v>
+      </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1281,13 +2714,13 @@
         <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s">
         <v>50</v>
       </c>
-      <c r="D18" t="s">
-        <v>51</v>
-      </c>
       <c r="E18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F18" t="str">
         <f>IF(H18&lt;B18, "n", "y")</f>
@@ -1312,10 +2745,43 @@
         <v>2</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="N18">
+        <v>28</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="W18">
+        <v>1</v>
+      </c>
+      <c r="X18" s="4" t="s">
+        <v>255</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1323,10 +2789,10 @@
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F19" t="str">
         <f>IF(H19&lt;B19, "n", "y")</f>
@@ -1351,10 +2817,43 @@
         <v>2</v>
       </c>
       <c r="M19" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="N19">
+        <v>26</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
+      <c r="V19" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="X19" s="4" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1362,10 +2861,10 @@
         <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F20" t="str">
         <f>IF(H20&lt;B20, "n", "y")</f>
@@ -1389,8 +2888,42 @@
       <c r="L20">
         <v>2</v>
       </c>
+      <c r="N20">
+        <f t="shared" ref="N18:N35" si="2">SUM(G20:L20)</f>
+        <v>23</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="U20">
+        <v>1</v>
+      </c>
+      <c r="V20" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20" s="4" t="s">
+        <v>257</v>
+      </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1398,13 +2931,13 @@
         <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F21" t="str">
         <f>IF(H21&lt;B21, "n", "y")</f>
@@ -1429,10 +2962,43 @@
         <v>2</v>
       </c>
       <c r="M21" t="s">
-        <v>91</v>
+        <v>89</v>
+      </c>
+      <c r="N21">
+        <v>28</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="W21">
+        <v>1</v>
+      </c>
+      <c r="X21" s="4" t="s">
+        <v>258</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1440,10 +3006,10 @@
         <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F22" t="str">
         <f>IF(H22&lt;B22, "n", "y")</f>
@@ -1468,10 +3034,43 @@
         <v>2</v>
       </c>
       <c r="M22" t="s">
-        <v>92</v>
+        <v>90</v>
+      </c>
+      <c r="N22">
+        <v>24</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="W22">
+        <v>1</v>
+      </c>
+      <c r="X22" s="4" t="s">
+        <v>259</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1479,13 +3078,13 @@
         <v>8</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" t="s">
         <v>54</v>
       </c>
-      <c r="D23" t="s">
-        <v>55</v>
-      </c>
       <c r="E23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F23" t="str">
         <f>IF(H23&lt;B23, "n", "y")</f>
@@ -1510,10 +3109,43 @@
         <v>2</v>
       </c>
       <c r="M23" t="s">
-        <v>93</v>
+        <v>91</v>
+      </c>
+      <c r="N23">
+        <v>28</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="T23" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="U23">
+        <v>1</v>
+      </c>
+      <c r="V23" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="W23">
+        <v>1</v>
+      </c>
+      <c r="X23" s="4" t="s">
+        <v>260</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1521,10 +3153,10 @@
         <v>14</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F24" t="str">
         <f>IF(H24&lt;B24, "n", "y")</f>
@@ -1549,10 +3181,43 @@
         <v>2</v>
       </c>
       <c r="M24" t="s">
-        <v>94</v>
+        <v>92</v>
+      </c>
+      <c r="N24">
+        <v>28</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="R24" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="T24" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="U24">
+        <v>1</v>
+      </c>
+      <c r="V24" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="W24">
+        <v>1</v>
+      </c>
+      <c r="X24" s="4" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1560,13 +3225,13 @@
         <v>8</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" t="s">
         <v>59</v>
       </c>
-      <c r="D25" t="s">
-        <v>60</v>
-      </c>
       <c r="E25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F25" t="str">
         <f>IF(H25&lt;B25, "n", "y")</f>
@@ -1591,10 +3256,43 @@
         <v>2</v>
       </c>
       <c r="M25" t="s">
-        <v>95</v>
+        <v>93</v>
+      </c>
+      <c r="N25">
+        <v>28</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+      <c r="R25" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="T25" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="U25">
+        <v>1</v>
+      </c>
+      <c r="V25" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="W25">
+        <v>1</v>
+      </c>
+      <c r="X25" s="4" t="s">
+        <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1602,10 +3300,10 @@
         <v>8</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F26" t="str">
         <f>IF(H26&lt;B26, "n", "y")</f>
@@ -1630,10 +3328,43 @@
         <v>2</v>
       </c>
       <c r="M26" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+      <c r="N26">
+        <v>23</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="R26" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="T26" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="U26">
+        <v>1</v>
+      </c>
+      <c r="V26" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="W26">
+        <v>1</v>
+      </c>
+      <c r="X26" s="4" t="s">
+        <v>263</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1641,10 +3372,10 @@
         <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F27" t="str">
         <f>IF(H27&lt;B27, "n", "y")</f>
@@ -1669,10 +3400,43 @@
         <v>2</v>
       </c>
       <c r="M27" t="s">
-        <v>97</v>
+        <v>95</v>
+      </c>
+      <c r="N27">
+        <v>25</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+      <c r="R27" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="S27">
+        <v>1</v>
+      </c>
+      <c r="T27" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="U27">
+        <v>1</v>
+      </c>
+      <c r="V27" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="W27">
+        <v>1</v>
+      </c>
+      <c r="X27" s="4" t="s">
+        <v>264</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1695,8 +3459,42 @@
       <c r="I28">
         <v>1</v>
       </c>
+      <c r="N28">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="R28" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="S28">
+        <v>1</v>
+      </c>
+      <c r="T28" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="U28">
+        <v>1</v>
+      </c>
+      <c r="V28" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="W28">
+        <v>1</v>
+      </c>
+      <c r="X28" s="4" t="s">
+        <v>265</v>
+      </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1719,8 +3517,42 @@
       <c r="I29">
         <v>1</v>
       </c>
+      <c r="N29">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q29">
+        <v>1</v>
+      </c>
+      <c r="R29" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="S29">
+        <v>1</v>
+      </c>
+      <c r="T29" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="U29">
+        <v>1</v>
+      </c>
+      <c r="V29" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="W29">
+        <v>1</v>
+      </c>
+      <c r="X29" s="4" t="s">
+        <v>266</v>
+      </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1743,8 +3575,42 @@
       <c r="I30">
         <v>1</v>
       </c>
+      <c r="N30">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O30">
+        <v>1</v>
+      </c>
+      <c r="P30" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q30">
+        <v>1</v>
+      </c>
+      <c r="R30" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
+      </c>
+      <c r="T30" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="U30">
+        <v>1</v>
+      </c>
+      <c r="V30" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="W30">
+        <v>1</v>
+      </c>
+      <c r="X30" s="4" t="s">
+        <v>267</v>
+      </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1752,13 +3618,13 @@
         <v>3</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E31" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" ref="F31:F35" si="1">IF(H31&lt;B31, "n", "y")</f>
+        <f t="shared" ref="F31:F35" si="3">IF(H31&lt;B31, "n", "y")</f>
         <v>y</v>
       </c>
       <c r="G31">
@@ -1779,8 +3645,42 @@
       <c r="L31">
         <v>2</v>
       </c>
+      <c r="N31">
+        <f>SUM(G31:L31)</f>
+        <v>15</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q31">
+        <v>1</v>
+      </c>
+      <c r="R31" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="S31">
+        <v>1</v>
+      </c>
+      <c r="T31" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+      <c r="V31" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="W31">
+        <v>1</v>
+      </c>
+      <c r="X31" s="4" t="s">
+        <v>268</v>
+      </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1788,13 +3688,13 @@
         <v>3</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>n</v>
       </c>
       <c r="G32">
@@ -1815,22 +3715,56 @@
       <c r="L32">
         <v>2</v>
       </c>
+      <c r="N32">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q32">
+        <v>1</v>
+      </c>
+      <c r="R32" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+      <c r="T32" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="U32">
+        <v>1</v>
+      </c>
+      <c r="V32" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="W32">
+        <v>1</v>
+      </c>
+      <c r="X32" s="4" t="s">
+        <v>269</v>
+      </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>292</v>
       </c>
       <c r="B33">
         <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>n</v>
       </c>
       <c r="G33">
@@ -1851,22 +3785,56 @@
       <c r="L33">
         <v>2</v>
       </c>
+      <c r="N33">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="O33">
+        <v>1</v>
+      </c>
+      <c r="P33" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q33">
+        <v>1</v>
+      </c>
+      <c r="R33" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="S33">
+        <v>1</v>
+      </c>
+      <c r="T33" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="U33">
+        <v>1</v>
+      </c>
+      <c r="V33" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="W33">
+        <v>1</v>
+      </c>
+      <c r="X33" s="4" t="s">
+        <v>270</v>
+      </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>7</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E34" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>n</v>
       </c>
       <c r="G34">
@@ -1888,24 +3856,57 @@
         <v>2</v>
       </c>
       <c r="M34" t="s">
-        <v>99</v>
+        <v>97</v>
+      </c>
+      <c r="N34">
+        <v>24</v>
+      </c>
+      <c r="O34">
+        <v>1</v>
+      </c>
+      <c r="P34" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q34">
+        <v>1</v>
+      </c>
+      <c r="R34" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="S34">
+        <v>1</v>
+      </c>
+      <c r="T34" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="U34">
+        <v>1</v>
+      </c>
+      <c r="V34" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="W34">
+        <v>1</v>
+      </c>
+      <c r="X34" s="4" t="s">
+        <v>271</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>7</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E35" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>n</v>
       </c>
       <c r="G35">
@@ -1927,10 +3928,83 @@
         <v>2</v>
       </c>
       <c r="M35" t="s">
-        <v>100</v>
+        <v>98</v>
+      </c>
+      <c r="N35">
+        <v>24</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+      <c r="P35" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q35">
+        <v>1</v>
+      </c>
+      <c r="R35" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="S35">
+        <v>1</v>
+      </c>
+      <c r="T35" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="U35">
+        <v>1</v>
+      </c>
+      <c r="V35" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="W35">
+        <v>1</v>
+      </c>
+      <c r="X35" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="N36" s="6">
+        <f>SUM(N2:N35)</f>
+        <v>707</v>
+      </c>
+      <c r="O36" s="6">
+        <f>SUM(O2:O35)</f>
+        <v>114</v>
+      </c>
+      <c r="Q36" s="6">
+        <f>SUM(Q2:Q35)</f>
+        <v>34</v>
+      </c>
+      <c r="S36" s="6">
+        <v>34</v>
+      </c>
+      <c r="U36" s="6">
+        <v>34</v>
+      </c>
+      <c r="W36" s="6">
+        <f>SUM(W2:W35)</f>
+        <v>34</v>
+      </c>
+      <c r="Y36" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" ht="29" x14ac:dyDescent="0.35">
+      <c r="N38" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="O38" s="7">
+        <f>SUM(N36:Y36)</f>
+        <v>962</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>